<commit_message>
Excel Project: Bike Sales Data Visualization
</commit_message>
<xml_diff>
--- a/Excel/Excel Charts Tutorial File.xlsx
+++ b/Excel/Excel Charts Tutorial File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dale/MyFiles/job/DataAnalyst/DataAnalysis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E29266-196D-9D40-B6EC-A34E29EDC0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DBD688-8428-0D47-9C3C-3C905E864624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="500" windowWidth="24660" windowHeight="15500" activeTab="1" xr2:uid="{03CEABDE-3C67-4836-9FDD-609F2D7E7F08}"/>
   </bookViews>
@@ -16844,7 +16844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B444C6-5638-496B-93B2-259D582C3A1D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="137" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>

</xml_diff>